<commit_message>
Spatial analytics, menu table popup, geo utils, deps
</commit_message>
<xml_diff>
--- a/my-app/public/Store Location Data/Sushi_Zanmai_Cleaned.xlsx
+++ b/my-app/public/Store Location Data/Sushi_Zanmai_Cleaned.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\NAZRIN\nazrins\Empire Sushi\Store Location Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\NAZRIN\nazrins\Empire Sushi\my-app\public\Store Location Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C750C619-BCD8-4E30-AD3F-19EEAE25E85D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50793357-4593-4AB9-A1EE-D9AA83161B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-852" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -292,9 +292,6 @@
     <t>Main Place Mall, USJ, Selangor</t>
   </si>
   <si>
-    <t>42.430597,-71.455611</t>
-  </si>
-  <si>
     <t>DPulze Shopping Centre, Cyberjaya, Selangor</t>
   </si>
   <si>
@@ -380,6 +377,9 @@
   </si>
   <si>
     <t>2.9707029421408757, 101.7131443802242</t>
+  </si>
+  <si>
+    <t>3.026641463411387, 101.58129299371657</t>
   </si>
 </sst>
 </file>
@@ -758,18 +758,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="36.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47.4140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -780,7 +780,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -791,7 +791,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -802,7 +802,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -813,7 +813,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -824,7 +824,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -835,7 +835,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -846,7 +846,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -857,7 +857,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -868,7 +868,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -879,7 +879,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -890,7 +890,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -901,7 +901,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -912,7 +912,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -923,7 +923,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -934,7 +934,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -945,7 +945,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -956,7 +956,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -967,7 +967,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -978,7 +978,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -989,7 +989,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>59</v>
       </c>
@@ -1000,7 +1000,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>62</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>65</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>68</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>71</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>74</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>77</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>80</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>83</v>
       </c>
@@ -1085,10 +1085,10 @@
         <v>84</v>
       </c>
       <c r="C29" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>85</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>88</v>
       </c>
@@ -1107,111 +1107,111 @@
         <v>89</v>
       </c>
       <c r="C31" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>116</v>
+      </c>
+      <c r="B32" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+      <c r="C32" t="s">
         <v>117</v>
       </c>
-      <c r="B32" t="s">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>91</v>
       </c>
-      <c r="C32" t="s">
+      <c r="B33" t="s">
+        <v>92</v>
+      </c>
+      <c r="C33" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>92</v>
-      </c>
-      <c r="B33" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>93</v>
       </c>
-      <c r="C33" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+      <c r="B34" t="s">
         <v>94</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>95</v>
       </c>
-      <c r="C34" t="s">
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+      <c r="B35" t="s">
         <v>97</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>98</v>
       </c>
-      <c r="C35" t="s">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+      <c r="B36" t="s">
         <v>100</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>101</v>
       </c>
-      <c r="C36" t="s">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+      <c r="B37" t="s">
         <v>103</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>104</v>
       </c>
-      <c r="C37" t="s">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+      <c r="B38" t="s">
         <v>106</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>107</v>
       </c>
-      <c r="C38" t="s">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+      <c r="B39" t="s">
         <v>109</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>110</v>
       </c>
-      <c r="C39" t="s">
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+      <c r="B40" t="s">
         <v>112</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>113</v>
       </c>
-      <c r="C40" t="s">
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>115</v>
       </c>
       <c r="B41" t="s">
         <v>75</v>
@@ -1223,7 +1223,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:C28 A30:C31 A29:B29 A34:C41 B32 A33:B33" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:C28 A30:C30 A29:B29 A34:C41 B32 A33:B33 B31" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>